<commit_message>
Implemented pojo for web tables user add, refactored code to use headers in excel file. Web table Add and search testing working
</commit_message>
<xml_diff>
--- a/TestData/Students_Details.xlsx
+++ b/TestData/Students_Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASN\eclipse_workspace\demoqa-automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A498C3-E4FE-4FD8-8F3A-781CD2C15988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24896B0F-49B3-4B4B-8D14-0389F9D2C388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>First Name</t>
   </si>
@@ -178,6 +178,27 @@
   </si>
   <si>
     <t>Sports,Reading</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Recreation</t>
   </si>
 </sst>
 </file>
@@ -518,10 +539,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,7 +561,7 @@
     <col min="12" max="12" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +598,17 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -615,8 +645,17 @@
       <c r="L2" t="s">
         <v>25</v>
       </c>
+      <c r="M2">
+        <v>34</v>
+      </c>
+      <c r="N2">
+        <v>28000</v>
+      </c>
+      <c r="O2" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -653,8 +692,17 @@
       <c r="L3" t="s">
         <v>27</v>
       </c>
+      <c r="M3">
+        <v>30</v>
+      </c>
+      <c r="N3">
+        <v>18000</v>
+      </c>
+      <c r="O3" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -691,8 +739,17 @@
       <c r="L4" t="s">
         <v>29</v>
       </c>
+      <c r="M4">
+        <v>40</v>
+      </c>
+      <c r="N4">
+        <v>15000</v>
+      </c>
+      <c r="O4" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -728,6 +785,15 @@
       </c>
       <c r="L5" t="s">
         <v>31</v>
+      </c>
+      <c r="M5">
+        <v>42</v>
+      </c>
+      <c r="N5">
+        <v>19000</v>
+      </c>
+      <c r="O5" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed URL Retry, Impletemed Assertions, Widget Auto Complete & Retry Failed Tests in progress
</commit_message>
<xml_diff>
--- a/TestData/Students_Details.xlsx
+++ b/TestData/Students_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASN\eclipse_workspace\demoqa-automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24896B0F-49B3-4B4B-8D14-0389F9D2C388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3839EBF5-F536-4D0A-80CC-3661171F63B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>First Name</t>
   </si>
@@ -199,6 +199,21 @@
   </si>
   <si>
     <t>Recreation</t>
+  </si>
+  <si>
+    <t>Current Address</t>
+  </si>
+  <si>
+    <t>301 Town 481, Brookville\n kansas 42129\n United States</t>
+  </si>
+  <si>
+    <t>302 Town 481, Brookville\n kansas 42129\n United States</t>
+  </si>
+  <si>
+    <t>303 Town 481, Brookville\n kansas 42129\n United States</t>
+  </si>
+  <si>
+    <t>304 Town 481, Brookville\n kansas 42129\n United States</t>
   </si>
 </sst>
 </file>
@@ -539,10 +554,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,17 +566,18 @@
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="50.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,22 +609,25 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -640,22 +659,25 @@
         <v>19</v>
       </c>
       <c r="K2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>34</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>28000</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -687,22 +709,25 @@
         <v>20</v>
       </c>
       <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
         <v>26</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>27</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>30</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>18000</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -734,22 +759,25 @@
         <v>21</v>
       </c>
       <c r="K4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" t="s">
         <v>28</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>29</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>40</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>15000</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -781,18 +809,21 @@
         <v>34</v>
       </c>
       <c r="K5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" t="s">
         <v>30</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>31</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>42</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>19000</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new column DOBTime
</commit_message>
<xml_diff>
--- a/TestData/Students_Details.xlsx
+++ b/TestData/Students_Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASN\eclipse_workspace\demoqa-automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3839EBF5-F536-4D0A-80CC-3661171F63B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C502D88-725A-40AC-82A6-EB97C63023BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>First Name</t>
   </si>
@@ -75,27 +75,15 @@
     <t>Accounting</t>
   </si>
   <si>
-    <t>Biology</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>511 Grant 481, Prattsville\n Arkansas 72129\n United States</t>
   </si>
   <si>
     <t>512 Grant 481, Prattsville\n Arkansas 72129\n United States</t>
   </si>
   <si>
-    <t>513 Grant 481, Prattsville\n Arkansas 72129\n United States</t>
-  </si>
-  <si>
-    <t>Reading</t>
-  </si>
-  <si>
     <t>/TestData/Mphoto.jpg</t>
   </si>
   <si>
@@ -111,45 +99,12 @@
     <t>Merrut</t>
   </si>
   <si>
-    <t>Haryana</t>
-  </si>
-  <si>
-    <t>Panipat</t>
-  </si>
-  <si>
-    <t>Rajasthan</t>
-  </si>
-  <si>
-    <t>Jaiselmer</t>
-  </si>
-  <si>
-    <t>Social Studies</t>
-  </si>
-  <si>
-    <t>/TestData/M2photo.jpg</t>
-  </si>
-  <si>
-    <t>514 Grant 481, Prattsville\n Arkansas 72129\n United States</t>
-  </si>
-  <si>
     <t>Gene</t>
   </si>
   <si>
-    <t>Bud</t>
-  </si>
-  <si>
-    <t>Wisem</t>
-  </si>
-  <si>
-    <t>Tom</t>
-  </si>
-  <si>
     <t>Femina</t>
   </si>
   <si>
-    <t>Boss</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -159,27 +114,15 @@
     <t>GFemina@demoqa.com</t>
   </si>
   <si>
-    <t>BWisem@demoqa.com</t>
-  </si>
-  <si>
-    <t>TBoss@demoqa.com</t>
-  </si>
-  <si>
     <t>/TestData/Fphoto.png</t>
   </si>
   <si>
-    <t>/TestData/Ophoto.jpg</t>
-  </si>
-  <si>
     <t>Sports,Music</t>
   </si>
   <si>
     <t>Music,Reading</t>
   </si>
   <si>
-    <t>Sports,Reading</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -195,12 +138,6 @@
     <t>Finance</t>
   </si>
   <si>
-    <t>Medicine</t>
-  </si>
-  <si>
-    <t>Recreation</t>
-  </si>
-  <si>
     <t>Current Address</t>
   </si>
   <si>
@@ -210,18 +147,16 @@
     <t>302 Town 481, Brookville\n kansas 42129\n United States</t>
   </si>
   <si>
-    <t>303 Town 481, Brookville\n kansas 42129\n United States</t>
-  </si>
-  <si>
-    <t>304 Town 481, Brookville\n kansas 42129\n United States</t>
+    <t>DOBTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -270,8 +205,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -554,10 +489,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,16 +503,18 @@
     <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="50.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="50.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -597,45 +534,48 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>58</v>
-      </c>
       <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
-        <v>51</v>
-      </c>
       <c r="O1" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="P1" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>42</v>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -646,49 +586,52 @@
       <c r="F2" s="1">
         <v>36753</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3">
+        <v>0.28125</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>48</v>
-      </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="L2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2">
+        <v>34</v>
+      </c>
+      <c r="P2">
+        <v>28000</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="M2" t="s">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="N2">
-        <v>34</v>
-      </c>
-      <c r="O2">
-        <v>28000</v>
-      </c>
-      <c r="P2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>43</v>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>1888343432</v>
@@ -696,147 +639,48 @@
       <c r="F3" s="1">
         <v>37398</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
-        <v>49</v>
-      </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3">
         <v>30</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>18000</v>
       </c>
-      <c r="P3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="Q3" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <v>8932465432</v>
-      </c>
-      <c r="F4" s="1">
-        <v>36525</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4">
-        <v>40</v>
-      </c>
-      <c r="O4">
-        <v>15000</v>
-      </c>
-      <c r="P4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>7839875281</v>
-      </c>
-      <c r="F5" s="2">
-        <v>37647</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5">
-        <v>42</v>
-      </c>
-      <c r="O5">
-        <v>19000</v>
-      </c>
-      <c r="P5" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{C2C45B91-D721-41D3-8067-48DAA8F27E7F}"/>
-    <hyperlink ref="C3:C5" r:id="rId2" display="Jbravo@demoqa.com" xr:uid="{02946429-FC30-4EC7-ADCA-DB69B93D14D8}"/>
+    <hyperlink ref="C3" r:id="rId2" display="Jbravo@demoqa.com" xr:uid="{02946429-FC30-4EC7-ADCA-DB69B93D14D8}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{4BF97F74-F741-4167-ADE1-FBDE5C06E711}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{EC7E2090-6981-4861-BB31-61C33EABC4E6}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{D64C00C7-C994-481B-9F9A-0F343AD53E37}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactore retryUrlAccess for server side errors, Refactored codes to support assertions for formspage and datepicker page
</commit_message>
<xml_diff>
--- a/TestData/Students_Details.xlsx
+++ b/TestData/Students_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASN\eclipse_workspace\demoqa-automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C502D88-725A-40AC-82A6-EB97C63023BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C04CDB5-F205-48A3-BF39-F45A97C3CA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>First Name</t>
   </si>
@@ -75,15 +75,27 @@
     <t>Accounting</t>
   </si>
   <si>
+    <t>Biology</t>
+  </si>
+  <si>
     <t>Female</t>
   </si>
   <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>511 Grant 481, Prattsville\n Arkansas 72129\n United States</t>
   </si>
   <si>
     <t>512 Grant 481, Prattsville\n Arkansas 72129\n United States</t>
   </si>
   <si>
+    <t>513 Grant 481, Prattsville\n Arkansas 72129\n United States</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
     <t>/TestData/Mphoto.jpg</t>
   </si>
   <si>
@@ -99,12 +111,45 @@
     <t>Merrut</t>
   </si>
   <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Panipat</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>Jaiselmer</t>
+  </si>
+  <si>
+    <t>Social Studies</t>
+  </si>
+  <si>
+    <t>/TestData/M2photo.jpg</t>
+  </si>
+  <si>
+    <t>514 Grant 481, Prattsville\n Arkansas 72129\n United States</t>
+  </si>
+  <si>
     <t>Gene</t>
   </si>
   <si>
+    <t>Bud</t>
+  </si>
+  <si>
+    <t>Wisem</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
     <t>Femina</t>
   </si>
   <si>
+    <t>Boss</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -114,15 +159,27 @@
     <t>GFemina@demoqa.com</t>
   </si>
   <si>
+    <t>BWisem@demoqa.com</t>
+  </si>
+  <si>
+    <t>TBoss@demoqa.com</t>
+  </si>
+  <si>
     <t>/TestData/Fphoto.png</t>
   </si>
   <si>
+    <t>/TestData/Ophoto.jpg</t>
+  </si>
+  <si>
     <t>Sports,Music</t>
   </si>
   <si>
     <t>Music,Reading</t>
   </si>
   <si>
+    <t>Sports,Reading</t>
+  </si>
+  <si>
     <t>Age</t>
   </si>
   <si>
@@ -138,6 +195,12 @@
     <t>Finance</t>
   </si>
   <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Recreation</t>
+  </si>
+  <si>
     <t>Current Address</t>
   </si>
   <si>
@@ -145,6 +208,12 @@
   </si>
   <si>
     <t>302 Town 481, Brookville\n kansas 42129\n United States</t>
+  </si>
+  <si>
+    <t>303 Town 481, Brookville\n kansas 42129\n United States</t>
+  </si>
+  <si>
+    <t>304 Town 481, Brookville\n kansas 42129\n United States</t>
   </si>
   <si>
     <t>DOBTime</t>
@@ -156,7 +225,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -202,11 +271,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -489,10 +559,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:Q3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +581,6 @@
     <col min="12" max="12" width="50.44140625" customWidth="1"/>
     <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -522,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -534,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -549,7 +618,7 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="M1" t="s">
         <v>9</v>
@@ -558,13 +627,13 @@
         <v>10</v>
       </c>
       <c r="O1" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="P1" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="Q1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -574,8 +643,8 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
+      <c r="C2" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -586,29 +655,29 @@
       <c r="F2" s="1">
         <v>36753</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>0.28125</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="O2">
         <v>34</v>
@@ -617,21 +686,21 @@
         <v>28000</v>
       </c>
       <c r="Q2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>1888343432</v>
@@ -639,29 +708,29 @@
       <c r="F3" s="1">
         <v>37398</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="4">
         <v>0.6875</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O3">
         <v>30</v>
@@ -670,17 +739,125 @@
         <v>18000</v>
       </c>
       <c r="Q3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>8932465432</v>
+      </c>
+      <c r="F4" s="1">
+        <v>36525</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4">
+        <v>40</v>
+      </c>
+      <c r="P4">
+        <v>15000</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>7839875281</v>
+      </c>
+      <c r="F5" s="2">
+        <v>37647</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" t="s">
+        <v>62</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5">
+        <v>42</v>
+      </c>
+      <c r="P5">
+        <v>19000</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{C2C45B91-D721-41D3-8067-48DAA8F27E7F}"/>
-    <hyperlink ref="C3" r:id="rId2" display="Jbravo@demoqa.com" xr:uid="{02946429-FC30-4EC7-ADCA-DB69B93D14D8}"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="Jbravo@demoqa.com" xr:uid="{02946429-FC30-4EC7-ADCA-DB69B93D14D8}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{4BF97F74-F741-4167-ADE1-FBDE5C06E711}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{EC7E2090-6981-4861-BB31-61C33EABC4E6}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{D64C00C7-C994-481B-9F9A-0F343AD53E37}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>